<commit_message>
fixed code trained model
</commit_message>
<xml_diff>
--- a/data/data_T1.xlsx
+++ b/data/data_T1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\מסמכים\ASE_audio\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Autism\ASD_estimation_Marina\Code\ASDSpeech\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762A8C2-BB68-40F3-9132-4433CE6A8436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,7 +342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,8 +369,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,32 +705,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="B1:B1048576 D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="4.44140625" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="9" max="10" width="8.33203125" customWidth="1"/>
-    <col min="11" max="11" width="8.21875" customWidth="1"/>
-    <col min="12" max="12" width="3.109375" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" customWidth="1"/>
-    <col min="14" max="14" width="3.21875" customWidth="1"/>
+    <col min="9" max="11" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
@@ -773,8 +772,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">
@@ -817,8 +816,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
@@ -861,8 +860,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B4" t="s">
@@ -905,8 +904,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B5" t="s">
@@ -949,8 +948,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B6" t="s">
@@ -993,8 +992,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B7" t="s">
@@ -1037,8 +1036,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B8" t="s">
@@ -1081,8 +1080,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
@@ -1125,8 +1124,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
@@ -1169,8 +1168,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B11" t="s">
@@ -1213,8 +1212,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B12" t="s">
@@ -1257,8 +1256,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B13" t="s">
@@ -1301,8 +1300,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B14" t="s">
@@ -1345,8 +1344,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B15" t="s">
@@ -1389,8 +1388,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B16" t="s">
@@ -1433,8 +1432,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B17" t="s">
@@ -1477,8 +1476,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B18" t="s">
@@ -1521,8 +1520,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B19" t="s">
@@ -1565,8 +1564,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B20" t="s">
@@ -1609,8 +1608,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B21" t="s">
@@ -1653,8 +1652,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B22" t="s">
@@ -1697,8 +1696,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B23" t="s">
@@ -1741,8 +1740,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B24" t="s">
@@ -1785,8 +1784,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B25" t="s">
@@ -1829,8 +1828,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B26" t="s">
@@ -1873,8 +1872,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B27" t="s">
@@ -1917,8 +1916,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B28" t="s">
@@ -1961,8 +1960,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B29" t="s">
@@ -2005,8 +2004,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B30" t="s">
@@ -2049,8 +2048,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B31" t="s">
@@ -2093,8 +2092,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B32" t="s">
@@ -2137,8 +2136,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B33" t="s">
@@ -2181,8 +2180,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B34" t="s">
@@ -2225,8 +2224,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B35" t="s">
@@ -2269,8 +2268,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B36" t="s">
@@ -2313,8 +2312,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B37" t="s">
@@ -2357,8 +2356,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B38" t="s">
@@ -2401,8 +2400,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B39" t="s">
@@ -2445,8 +2444,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B40" t="s">
@@ -2489,8 +2488,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B41" t="s">
@@ -2533,8 +2532,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B42" t="s">
@@ -2577,8 +2576,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B43" t="s">
@@ -2621,8 +2620,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B44" t="s">
@@ -2665,8 +2664,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B45" t="s">
@@ -2709,8 +2708,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B46" t="s">
@@ -2753,8 +2752,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B47" t="s">
@@ -2797,8 +2796,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B48" t="s">
@@ -2841,8 +2840,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B49" t="s">
@@ -2885,8 +2884,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B50" t="s">
@@ -2929,8 +2928,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B51" t="s">
@@ -2973,8 +2972,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B52" t="s">
@@ -3017,8 +3016,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B53" t="s">
@@ -3061,8 +3060,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B54" t="s">
@@ -3105,8 +3104,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B55" t="s">
@@ -3149,8 +3148,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B56" t="s">
@@ -3193,8 +3192,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B57" t="s">
@@ -3237,8 +3236,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B58" t="s">
@@ -3281,8 +3280,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B59" t="s">
@@ -3325,8 +3324,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B60" t="s">
@@ -3369,8 +3368,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B61" t="s">
@@ -3413,8 +3412,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B62" t="s">
@@ -3459,5 +3458,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A25" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>